<commit_message>
Initial commit; added scripts, notebooks and models
</commit_message>
<xml_diff>
--- a/df_processed.xlsx
+++ b/df_processed.xlsx
@@ -37903,175 +37903,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063EC4F616B0A044F9A9B9014E3F277BF" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a8032452de733b8d12c1ee4f448036d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48343f2e-c123-49f7-ba03-78ca39fc17ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91a3a6ae5934e6b4bd6374ecb6b5c468" ns2:_="">
-    <xsd:import namespace="48343f2e-c123-49f7-ba03-78ca39fc17ff"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="48343f2e-c123-49f7-ba03-78ca39fc17ff" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98D14740-0843-41BB-BDE3-0FB7C13F0A76}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BD0B5BE-EDA2-4E2F-B170-31F26C91E449}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E9CFB-3ACA-4426-94F8-0830AF31FC91}"/>
 </file>
</xml_diff>